<commit_message>
June update, commented out deflator pull
</commit_message>
<xml_diff>
--- a/data/monthly_state_employment.xlsx
+++ b/data/monthly_state_employment.xlsx
@@ -1,21 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsalwati\Downloads\Hutchins Fiscal Impact Measure\fim\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F11E80C-7CBD-4711-AA09-3384790FD320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Haver code</t>
+  </si>
+  <si>
+    <t>Jan-21</t>
+  </si>
+  <si>
+    <t>Feb-21</t>
+  </si>
+  <si>
+    <t>Mar-21</t>
+  </si>
+  <si>
+    <t>Apr-21</t>
+  </si>
+  <si>
+    <t>May-21</t>
+  </si>
+  <si>
+    <t>Jun-21</t>
+  </si>
+  <si>
+    <t>Jul-21</t>
+  </si>
+  <si>
+    <t>Aug-21</t>
+  </si>
+  <si>
+    <t>Sep-21</t>
+  </si>
+  <si>
+    <t>Oct-21</t>
+  </si>
+  <si>
+    <t>Nov-21</t>
+  </si>
+  <si>
+    <t>Dec-21</t>
+  </si>
+  <si>
+    <t>Jan-22</t>
+  </si>
+  <si>
+    <t>Feb-22</t>
+  </si>
+  <si>
+    <t>Mar-22</t>
+  </si>
+  <si>
+    <t>lasgova</t>
+  </si>
+  <si>
+    <t>lalgova</t>
+  </si>
+  <si>
+    <t>cpgs</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -30,6 +109,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,9 +137,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -63,6 +155,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -109,7 +209,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +241,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +293,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,100 +486,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Haver code</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Jan-21</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Feb-21</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Mar-21</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Apr-21</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>May-21</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Jun-21</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Jul-21</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Aug-21</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Sep-21</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Oct-21</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Nov-21</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Dec-21</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Jan-22</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Feb-22</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Mar-22</t>
-        </is>
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>44652</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>lasgova</t>
-        </is>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
       </c>
       <c r="B2">
         <v>5154</v>
@@ -482,20 +589,21 @@
         <v>5237</v>
       </c>
       <c r="N2">
-        <v>5219</v>
+        <v>5212</v>
       </c>
       <c r="O2">
-        <v>5207</v>
+        <v>5213</v>
       </c>
       <c r="P2">
-        <v>5193</v>
+        <v>5224</v>
+      </c>
+      <c r="Q2">
+        <v>5260</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>lalgova</t>
-        </is>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
       </c>
       <c r="B3">
         <v>13748</v>
@@ -537,17 +645,18 @@
         <v>14055</v>
       </c>
       <c r="O3">
-        <v>14076</v>
+        <v>14073</v>
       </c>
       <c r="P3">
-        <v>14096</v>
+        <v>14087</v>
+      </c>
+      <c r="Q3">
+        <v>14108</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>cpgs</t>
-        </is>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
       </c>
       <c r="B4">
         <v>328517</v>
@@ -585,14 +694,21 @@
       <c r="M4">
         <v>323714</v>
       </c>
-      <c r="N4">
-        <v>324157</v>
-      </c>
-      <c r="O4">
-        <v>323092</v>
+      <c r="N4" s="2">
+        <v>323638</v>
+      </c>
+      <c r="O4" s="3">
+        <v>324761</v>
+      </c>
+      <c r="P4" s="2">
+        <v>325304</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>323956</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
July update, incorporate MPI
</commit_message>
<xml_diff>
--- a/data/monthly_state_employment.xlsx
+++ b/data/monthly_state_employment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsalwati\Downloads\Hutchins Fiscal Impact Measure\fim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F11E80C-7CBD-4711-AA09-3384790FD320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41BA9F9-D844-4870-8252-91819FDC6C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,15 +487,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,8 +547,14 @@
       <c r="Q1" s="4">
         <v>44652</v>
       </c>
+      <c r="R1" s="4">
+        <v>44682</v>
+      </c>
+      <c r="S1" s="4">
+        <v>44713</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -598,10 +604,16 @@
         <v>5224</v>
       </c>
       <c r="Q2">
-        <v>5260</v>
+        <v>5218</v>
+      </c>
+      <c r="R2">
+        <v>5254</v>
+      </c>
+      <c r="S2">
+        <v>5253</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -651,10 +663,16 @@
         <v>14087</v>
       </c>
       <c r="Q3">
-        <v>14108</v>
+        <v>14091</v>
+      </c>
+      <c r="R3">
+        <v>14104</v>
+      </c>
+      <c r="S3">
+        <v>14109</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -701,10 +719,13 @@
         <v>324761</v>
       </c>
       <c r="P4" s="2">
-        <v>325304</v>
+        <v>319759</v>
       </c>
       <c r="Q4" s="2">
-        <v>323956</v>
+        <v>319650</v>
+      </c>
+      <c r="R4" s="2">
+        <v>317251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
September forecast sheet updates
Pushing September updates to forecast sheet. New data, MPI, etc.
</commit_message>
<xml_diff>
--- a/data/monthly_state_employment.xlsx
+++ b/data/monthly_state_employment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsalwati\Downloads\Hutchins Fiscal Impact Measure\fim\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EAsdourian\Desktop\Hutchins Centerfim\fim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41BA9F9-D844-4870-8252-91819FDC6C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A70F89-51F9-4E58-BB35-0E334A1E9E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2270" yWindow="690" windowWidth="19190" windowHeight="10190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,15 +487,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,8 +553,17 @@
       <c r="S1" s="4">
         <v>44713</v>
       </c>
+      <c r="T1" s="4">
+        <v>44743</v>
+      </c>
+      <c r="U1" s="4">
+        <v>44774</v>
+      </c>
+      <c r="V1" s="4">
+        <v>44805</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -595,25 +604,34 @@
         <v>5237</v>
       </c>
       <c r="N2">
+        <v>5219</v>
+      </c>
+      <c r="O2">
         <v>5212</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>5213</v>
-      </c>
-      <c r="P2">
-        <v>5224</v>
       </c>
       <c r="Q2">
         <v>5218</v>
       </c>
       <c r="R2">
-        <v>5254</v>
+        <v>5258</v>
       </c>
       <c r="S2">
-        <v>5253</v>
+        <v>5238</v>
+      </c>
+      <c r="T2">
+        <v>5246</v>
+      </c>
+      <c r="U2">
+        <v>5247</v>
+      </c>
+      <c r="V2">
+        <v>5231</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -666,13 +684,22 @@
         <v>14091</v>
       </c>
       <c r="R3">
-        <v>14104</v>
+        <v>14105</v>
       </c>
       <c r="S3">
-        <v>14109</v>
+        <v>14084</v>
+      </c>
+      <c r="T3">
+        <v>14157</v>
+      </c>
+      <c r="U3">
+        <v>14198</v>
+      </c>
+      <c r="V3">
+        <v>14187</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -726,6 +753,15 @@
       </c>
       <c r="R4" s="2">
         <v>317251</v>
+      </c>
+      <c r="S4" s="2">
+        <v>324999</v>
+      </c>
+      <c r="T4" s="2">
+        <v>331601</v>
+      </c>
+      <c r="U4" s="2">
+        <v>330337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>